<commit_message>
changes for exel util
</commit_message>
<xml_diff>
--- a/resources/profile.xlsx
+++ b/resources/profile.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="28695" windowHeight="13290"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="28695" windowHeight="13290" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="profile" sheetId="1" r:id="rId1"/>
+    <sheet name="password" sheetId="2" r:id="rId2"/>
+    <sheet name="notification" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>visible</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -260,7 +263,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -270,6 +273,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -565,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.140625" defaultRowHeight="20.25" customHeight="1"/>
@@ -763,287 +769,6 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="20.25" customHeight="1">
-      <c r="B19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
@@ -1055,24 +780,418 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="27" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="27" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2"/>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45">
+      <c r="A8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9"/>
+      <c r="B9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="60">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45">
+      <c r="A11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update profile for changes
</commit_message>
<xml_diff>
--- a/resources/profile.xlsx
+++ b/resources/profile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="28695" windowHeight="13290" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="28695" windowHeight="13290" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="profile" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>visible</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -571,13 +574,14 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.140625" defaultRowHeight="20.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="59.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" customHeight="1">
@@ -620,7 +624,7 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20.25" customHeight="1">
@@ -779,13 +783,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="27" style="5"/>
+    <col min="1" max="1" width="27" style="5"/>
+    <col min="2" max="2" width="65.5703125" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="27" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -829,7 +835,7 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -864,7 +870,7 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E4"/>
       <c r="F4"/>
@@ -968,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1014,7 +1020,7 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7">

</xml_diff>

<commit_message>
fix for clinician and profile
</commit_message>
<xml_diff>
--- a/resources/profile.xlsx
+++ b/resources/profile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="28695" windowHeight="13290" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="28695" windowHeight="13290" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="profile" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -141,12 +141,6 @@
     <t>a@gmail.com</t>
   </si>
   <si>
-    <t>/html/body/div[3]/md-dialog/md-dialog-actions/button[2]</t>
-  </si>
-  <si>
-    <t>//button[@ng-click="vm.go('triangular.profile')"]</t>
-  </si>
-  <si>
     <t>//input[@ng-model="vm.userSetting.address.address"]</t>
   </si>
   <si>
@@ -174,9 +168,6 @@
     <t>(//button[@class="md-raised md-primary margin-left-0 md-button ng-scope md-cs-content-theme-theme md-ink-ripple"])[1]</t>
   </si>
   <si>
-    <t>(//button[@class="md-raised md-primary margin-left-0 md-button ng-scope md-cs-content-theme-theme md-ink-ripple"])[2]</t>
-  </si>
-  <si>
     <t>(//button[@class="md-raised md-primary margin-left-0 md-button ng-scope md-cs-content-theme-theme md-ink-ripple"])[3]</t>
   </si>
   <si>
@@ -210,9 +201,6 @@
     <t>visible</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>Error</t>
   </si>
   <si>
@@ -223,6 +211,18 @@
   </si>
   <si>
     <t>Fail to update profile notification</t>
+  </si>
+  <si>
+    <t>//button[@ng-click="$mdOpenMenu($event)"]</t>
+  </si>
+  <si>
+    <t>//button[@ng-click="vm.openProfileEdit()"]</t>
+  </si>
+  <si>
+    <t>//button[@aria-label="Update Password"]</t>
+  </si>
+  <si>
+    <t>//button[@aria-label="Confirm!"]</t>
   </si>
 </sst>
 </file>
@@ -583,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.140625" defaultRowHeight="20.25" customHeight="1"/>
@@ -622,7 +622,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.25" customHeight="1">
@@ -630,7 +630,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -645,117 +645,117 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="20.25" customHeight="1">
+      <c r="B3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="20.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
       <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" t="s">
-        <v>66</v>
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="20.25" customHeight="1">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="20.25" customHeight="1">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
-        <v>37</v>
+      <c r="D5" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="J5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="20.25" customHeight="1">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>38</v>
+      <c r="D6" t="s">
+        <v>37</v>
       </c>
       <c r="J6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="20.25" customHeight="1">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="3">
-        <v>95901</v>
+      <c r="D7" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="J7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="20.25" customHeight="1">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>39</v>
+      <c r="D8" s="3">
+        <v>95901</v>
       </c>
       <c r="J8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="20.25" customHeight="1">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
@@ -764,66 +764,83 @@
         <v>39</v>
       </c>
       <c r="J9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="20.25" customHeight="1">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>40</v>
+      <c r="D10" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="J10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="20.25" customHeight="1">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="20.25" customHeight="1">
+      <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="20.25" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" t="s">
-        <v>66</v>
+    </row>
+    <row r="13" spans="1:10" ht="20.25" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1"/>
+    <hyperlink ref="D11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -832,10 +849,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27" defaultRowHeight="15"/>
@@ -872,20 +889,19 @@
         <v>6</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" customFormat="1" ht="20.25" customHeight="1">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2"/>
       <c r="E2">
         <v>1</v>
       </c>
@@ -893,23 +909,19 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" customFormat="1" ht="20.25" customHeight="1">
       <c r="B3" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3"/>
       <c r="E3">
         <v>1</v>
       </c>
@@ -917,102 +929,99 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
+        <v>7</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
       <c r="J4" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5"/>
       <c r="J5" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
       <c r="J6" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="J7" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7"/>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="J7" s="5" t="s">
+      <c r="B8" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -1028,37 +1037,63 @@
         <v>1</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9"/>
+      <c r="A9" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="B9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10"/>
+      <c r="B10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="56.5703125" customWidth="1"/>
     <col min="10" max="10" width="33.5703125" customWidth="1"/>
   </cols>
@@ -1086,12 +1121,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" ht="20.25" customHeight="1">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1103,18 +1138,15 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="20.25" customHeight="1">
       <c r="B3" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -1126,18 +1158,15 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -1152,15 +1181,15 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1175,15 +1204,15 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -1198,15 +1227,15 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -1221,15 +1250,15 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -1244,15 +1273,15 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -1267,44 +1296,67 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="45">
-      <c r="A11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>63</v>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>68</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>